<commit_message>
Proposal Version 1.0 plus addson
</commit_message>
<xml_diff>
--- a/Burndown.xlsx
+++ b/Burndown.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1989s\study\LastYear\CAPSTONE\proposal\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2356286F-78B5-4455-8A48-329D0BD67A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8371BE-0047-4784-AB11-AA9EEE4B0D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar" sheetId="12" r:id="rId1"/>
     <sheet name="Burndown" sheetId="13" r:id="rId2"/>
+    <sheet name="Change of Circumstances" sheetId="14" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="Holidays">[1]Holidays!$A$2:$A$23</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>Planned</t>
   </si>
@@ -94,9 +95,6 @@
     <t>Academic Hours</t>
   </si>
   <si>
-    <t>Break</t>
-  </si>
-  <si>
     <t>Industry Hours</t>
   </si>
   <si>
@@ -118,26 +116,50 @@
     <t xml:space="preserve">Color code </t>
   </si>
   <si>
-    <t>academic break</t>
-  </si>
-  <si>
     <t>Danger zone - final two weeks.</t>
   </si>
   <si>
-    <t>Color code</t>
+    <t>change of circumstances</t>
   </si>
   <si>
-    <t>Start or end of a phase</t>
+    <t>BIGGER FONT</t>
   </si>
   <si>
-    <t>Academic break</t>
+    <t>Special designations</t>
+  </si>
+  <si>
+    <t>ID - 2</t>
+  </si>
+  <si>
+    <t>ID-1</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Overfulfilled / underfulfilled the plan</t>
+  </si>
+  <si>
+    <t>An explanation of the difference between planned and actual time expenditure will be presented here.Note : Only significant situations with a time difference of at least 2 hours will be considered.</t>
+  </si>
+  <si>
+    <t>Overfulfilled</t>
+  </si>
+  <si>
+    <t>The project was found in a short time, it became possible to get to know the project, the company and the team earlier.</t>
+  </si>
+  <si>
+    <t>Acquaintance with the project took place earlier and faster than planned, there was no point in postponing the writing of the proposal for later. "Strike while the iron is hot".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,8 +233,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,12 +295,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -281,19 +319,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,8 +329,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF7FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -500,7 +532,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -512,6 +544,80 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -527,26 +633,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -555,85 +648,77 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -645,16 +730,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -670,22 +755,10 @@
     <xf numFmtId="16" fontId="1" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -726,129 +799,191 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="13" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="13" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,8 +994,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFEBF7FF"/>
       <color rgb="FFCCECFF"/>
-      <color rgb="FFEBF7FF"/>
       <color rgb="FFCC99FF"/>
       <color rgb="FFFF9900"/>
       <color rgb="FFCC0099"/>
@@ -967,7 +1102,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Burndown!$E$4</c:f>
+              <c:f>Burndown!$F$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1003,7 +1138,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Burndown!$B$5:$B$23</c:f>
+              <c:f>Burndown!$C$5:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1069,7 +1204,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$E$5:$E$23</c:f>
+              <c:f>Burndown!$F$5:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1145,7 +1280,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Burndown!$F$4</c:f>
+              <c:f>Burndown!$G$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1180,7 +1315,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Burndown!$B$5:$B$23</c:f>
+              <c:f>Burndown!$C$5:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1246,7 +1381,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$F$5:$F$23</c:f>
+              <c:f>Burndown!$G$5:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1260,52 +1395,10 @@
                   <c:v>114.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>107.5</c:v>
+                  <c:v>104.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>107.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>107.5</c:v>
+                  <c:v>95.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1724,7 +1817,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Burndown!$E$28</c:f>
+              <c:f>Burndown!$F$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1757,7 +1850,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Burndown!$B$29:$B$45</c:f>
+              <c:f>Burndown!$C$29:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1817,7 +1910,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$E$29:$E$45</c:f>
+              <c:f>Burndown!$F$29:$F$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1831,46 +1924,46 @@
                   <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>278</c:v>
+                  <c:v>290</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>256</c:v>
+                  <c:v>268</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>234</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>212</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>190</c:v>
+                  <c:v>202</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>168</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>147</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>126</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>105</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>84</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>63</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1887,7 +1980,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Burndown!$F$28</c:f>
+              <c:f>Burndown!$G$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1946,7 +2039,7 @@
           </c:dPt>
           <c:cat>
             <c:numRef>
-              <c:f>Burndown!$B$29:$B$45</c:f>
+              <c:f>Burndown!$C$29:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2006,7 +2099,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$F$29:$F$45</c:f>
+              <c:f>Burndown!$G$29:$G$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -3455,16 +3548,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>198120</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>370478</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:rowOff>14151</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>598715</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>75111</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3491,13 +3584,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>362857</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>586740</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
@@ -3926,7 +4019,7 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3947,52 +4040,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="28.5" x14ac:dyDescent="0.65">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
     </row>
     <row r="2" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="S2" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" s="66"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="S2" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="38"/>
     </row>
     <row r="3" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -4019,7 +4112,7 @@
       <c r="H3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="39"/>
+      <c r="I3" s="46"/>
       <c r="J3" s="2" t="s">
         <v>8</v>
       </c>
@@ -4043,86 +4136,110 @@
       </c>
       <c r="Q3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="S3" s="63"/>
-      <c r="T3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>45131</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="23">
         <v>3</v>
       </c>
-      <c r="C4" s="17">
-        <v>0</v>
-      </c>
-      <c r="D4" s="17">
+      <c r="C4" s="13">
+        <v>0</v>
+      </c>
+      <c r="D4" s="13">
         <v>1</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="13">
         <v>3</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="14">
         <v>1</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="13">
         <v>3</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="14">
         <v>3</v>
       </c>
-      <c r="I4" s="39"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="18"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="23">
+        <v>0</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0</v>
+      </c>
+      <c r="L4" s="13">
+        <v>0</v>
+      </c>
+      <c r="M4" s="13">
+        <v>0</v>
+      </c>
+      <c r="N4" s="14">
+        <v>0</v>
+      </c>
+      <c r="O4" s="13">
+        <v>0</v>
+      </c>
+      <c r="P4" s="14">
+        <v>0</v>
+      </c>
       <c r="Q4" s="6">
         <v>1</v>
       </c>
-      <c r="S4" s="64"/>
+      <c r="S4" s="36"/>
       <c r="T4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>45138</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="15">
         <v>2</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="16">
         <v>4</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="15">
         <v>4</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="17">
         <v>5</v>
       </c>
-      <c r="F5" s="22">
-        <v>0</v>
-      </c>
-      <c r="G5" s="21">
+      <c r="F5" s="18">
+        <v>0</v>
+      </c>
+      <c r="G5" s="17">
         <v>3</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="18">
         <v>3.5</v>
       </c>
-      <c r="I5" s="39"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="22"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="15">
+        <v>5</v>
+      </c>
+      <c r="K5" s="16">
+        <v>1</v>
+      </c>
+      <c r="L5" s="15">
+        <v>0</v>
+      </c>
+      <c r="M5" s="17">
+        <v>0</v>
+      </c>
+      <c r="N5" s="18">
+        <v>0</v>
+      </c>
+      <c r="O5" s="17">
+        <v>0</v>
+      </c>
+      <c r="P5" s="18">
+        <v>0</v>
+      </c>
       <c r="Q5" s="7">
         <v>2</v>
       </c>
@@ -4131,29 +4248,49 @@
       <c r="A6" s="9">
         <v>45145</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="17">
         <v>2</v>
       </c>
-      <c r="C6" s="21">
-        <v>0</v>
-      </c>
-      <c r="D6" s="21">
-        <v>0</v>
-      </c>
-      <c r="E6" s="21">
+      <c r="C6" s="17">
+        <v>0</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0</v>
+      </c>
+      <c r="E6" s="17">
         <v>5</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="22"/>
+      <c r="F6" s="18">
+        <v>0</v>
+      </c>
+      <c r="G6" s="17">
+        <v>0</v>
+      </c>
+      <c r="H6" s="18">
+        <v>3</v>
+      </c>
+      <c r="I6" s="46"/>
+      <c r="J6" s="17">
+        <v>0</v>
+      </c>
+      <c r="K6" s="17">
+        <v>5</v>
+      </c>
+      <c r="L6" s="17">
+        <v>0</v>
+      </c>
+      <c r="M6" s="17">
+        <v>0</v>
+      </c>
+      <c r="N6" s="18">
+        <v>0</v>
+      </c>
+      <c r="O6" s="17">
+        <v>0</v>
+      </c>
+      <c r="P6" s="18">
+        <v>0</v>
+      </c>
       <c r="Q6" s="7">
         <v>3</v>
       </c>
@@ -4162,21 +4299,41 @@
       <c r="A7" s="9">
         <v>45152</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="22"/>
+      <c r="B7" s="17">
+        <v>5</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0</v>
+      </c>
+      <c r="E7" s="17">
+        <v>4</v>
+      </c>
+      <c r="F7" s="18">
+        <v>0</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="17">
+        <v>0</v>
+      </c>
+      <c r="K7" s="17">
+        <v>0</v>
+      </c>
+      <c r="L7" s="18">
+        <v>0</v>
+      </c>
+      <c r="M7" s="17">
+        <v>3</v>
+      </c>
+      <c r="N7" s="18">
+        <v>0</v>
+      </c>
+      <c r="O7" s="17"/>
+      <c r="P7" s="18"/>
       <c r="Q7" s="7">
         <v>4</v>
       </c>
@@ -4185,21 +4342,21 @@
       <c r="A8" s="9">
         <v>45159</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="22"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="18"/>
       <c r="Q8" s="7">
         <v>5</v>
       </c>
@@ -4208,21 +4365,21 @@
       <c r="A9" s="9">
         <v>45166</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="22"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="18"/>
       <c r="Q9" s="7">
         <v>6</v>
       </c>
@@ -4231,21 +4388,21 @@
       <c r="A10" s="9">
         <v>45173</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="22"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="18"/>
       <c r="Q10" s="7">
         <v>7</v>
       </c>
@@ -4254,45 +4411,45 @@
       <c r="A11" s="9">
         <v>45180</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="22"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="18"/>
       <c r="Q11" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>45187</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="49">
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="7">
         <v>9</v>
       </c>
     </row>
@@ -4300,67 +4457,67 @@
       <c r="A13" s="9">
         <v>45194</v>
       </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="61"/>
-      <c r="Q13" s="50" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>45201</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="58"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="58"/>
-      <c r="O14" s="59"/>
-      <c r="P14" s="62"/>
-      <c r="Q14" s="51" t="s">
-        <v>17</v>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="7">
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>45208</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="18"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="14"/>
       <c r="Q15" s="6">
         <v>10</v>
       </c>
@@ -4369,21 +4526,21 @@
       <c r="A16" s="9">
         <v>45215</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="22"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="18"/>
       <c r="Q16" s="7">
         <v>11</v>
       </c>
@@ -4392,21 +4549,21 @@
       <c r="A17" s="9">
         <v>45222</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="22"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="18"/>
       <c r="Q17" s="7">
         <v>12</v>
       </c>
@@ -4415,21 +4572,21 @@
       <c r="A18" s="9">
         <v>45229</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="22"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="18"/>
       <c r="Q18" s="7">
         <v>13</v>
       </c>
@@ -4438,21 +4595,21 @@
       <c r="A19" s="9">
         <v>45236</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="22"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="18"/>
       <c r="Q19" s="7">
         <v>14</v>
       </c>
@@ -4461,21 +4618,21 @@
       <c r="A20" s="9">
         <v>45243</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="22"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="18"/>
       <c r="Q20" s="7">
         <v>15</v>
       </c>
@@ -4484,21 +4641,21 @@
       <c r="A21" s="9">
         <v>45250</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
       <c r="Q21" s="7">
         <v>16</v>
       </c>
@@ -4507,21 +4664,21 @@
       <c r="A22" s="9">
         <v>45257</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
       <c r="Q22" s="7">
         <v>17</v>
       </c>
@@ -4540,1026 +4697,1213 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F346F8-B11F-46DD-B3FE-6347E11FF9F9}">
-  <dimension ref="A1:S48"/>
+  <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="19" max="19" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="26" x14ac:dyDescent="0.6">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:22" ht="26" x14ac:dyDescent="0.6">
+      <c r="B1" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+    </row>
+    <row r="2" spans="1:22" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-    </row>
-    <row r="2" spans="1:19" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="41" t="s">
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B3" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="53"/>
+      <c r="D3" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="52"/>
+      <c r="F3" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="42"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="G3" s="52"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>0</v>
-      </c>
       <c r="D4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="10">
+    <row r="5" spans="1:22" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="59">
         <v>1</v>
       </c>
-      <c r="B5" s="11">
+      <c r="C5" s="57">
         <v>45131</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>12</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <f>SUM(Calendar!B4:H4)</f>
         <v>14</v>
       </c>
-      <c r="E5" s="1">
-        <f>C24</f>
+      <c r="F5" s="1">
+        <f>D24</f>
         <v>150</v>
       </c>
-      <c r="F5" s="1">
-        <f>C24</f>
+      <c r="G5" s="1">
+        <f>D24</f>
         <v>150</v>
       </c>
-      <c r="R5" s="69" t="s">
+      <c r="S5" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="S5" s="69"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="10">
+      <c r="T5" s="62"/>
+      <c r="U5" s="62"/>
+      <c r="V5" s="63"/>
+    </row>
+    <row r="6" spans="1:22" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="82">
         <v>2</v>
       </c>
-      <c r="B6" s="11">
+      <c r="C6" s="58">
         <v>45138</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>12</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <f>SUM(Calendar!B5:H5)</f>
         <v>21.5</v>
       </c>
-      <c r="E6" s="1">
-        <f>E5-C5</f>
-        <v>138</v>
-      </c>
       <c r="F6" s="1">
         <f>F5-D5</f>
+        <v>138</v>
+      </c>
+      <c r="G6" s="1">
+        <f>G5-E5</f>
         <v>136</v>
       </c>
-      <c r="R6" s="70"/>
-      <c r="S6" s="69" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="10">
+      <c r="S6" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="T6" s="64" t="s">
+        <v>25</v>
+      </c>
+      <c r="U6" s="65"/>
+      <c r="V6" s="66"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B7" s="60">
         <v>3</v>
       </c>
-      <c r="B7" s="11">
+      <c r="C7" s="58">
         <v>45145</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>12</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <f>SUM(Calendar!B6:H6)</f>
-        <v>7</v>
-      </c>
-      <c r="E7" s="1">
-        <f>E6-C6</f>
-        <v>126</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1">
         <f>F6-D6</f>
+        <v>126</v>
+      </c>
+      <c r="G7" s="1">
+        <f>G6-E6</f>
         <v>114.5</v>
       </c>
-      <c r="R7" s="74"/>
-      <c r="S7" s="69" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="10">
+      <c r="S7" s="32"/>
+      <c r="T7" s="65"/>
+      <c r="U7" s="65"/>
+      <c r="V7" s="66"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B8" s="60">
         <v>4</v>
       </c>
-      <c r="B8" s="11">
+      <c r="C8" s="57">
         <v>45152</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>12</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <f>SUM(Calendar!B7:H7)</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" ref="E8:E23" si="0">E7-C7</f>
+        <v>9</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" ref="F8:F23" si="0">F7-D7</f>
         <v>114</v>
       </c>
-      <c r="F8" s="1">
-        <f t="shared" ref="F8:F23" si="1">F7-D7</f>
-        <v>107.5</v>
-      </c>
-      <c r="R8" s="14"/>
-      <c r="S8" s="69" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="68">
+      <c r="G8" s="1">
+        <f t="shared" ref="G8:G9" si="1">G7-E7</f>
+        <v>104.5</v>
+      </c>
+      <c r="S8" s="67"/>
+      <c r="T8" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="U8" s="69"/>
+      <c r="V8" s="70"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B9" s="56">
         <v>5</v>
       </c>
-      <c r="B9" s="11">
+      <c r="C9" s="57">
         <v>45159</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>3</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <f>SUM(Calendar!B8:H8)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="10">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B10" s="56">
         <v>6</v>
       </c>
-      <c r="B10" s="11">
+      <c r="C10" s="57">
         <v>45166</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>3</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <f>SUM(Calendar!B9:H9)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="F10" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="10">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B11" s="56">
         <v>7</v>
       </c>
-      <c r="B11" s="11">
+      <c r="C11" s="57">
         <v>45173</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>3</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <f>SUM(Calendar!B10:H10)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="F11" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="10">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B12" s="56">
         <v>8</v>
       </c>
-      <c r="B12" s="11">
+      <c r="C12" s="57">
         <v>45180</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>3</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <f>SUM(Calendar!B11:H11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="F12" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="10">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B13" s="56">
         <v>9</v>
       </c>
-      <c r="B13" s="11">
+      <c r="C13" s="57">
         <v>45187</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>3</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <f>SUM(Calendar!B12:H12)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="F13" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="11">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B14" s="56">
+        <v>11</v>
+      </c>
+      <c r="C14" s="57">
         <v>45194</v>
       </c>
-      <c r="C14" s="14">
+      <c r="D14" s="42">
         <v>6</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <f>SUM(Calendar!B13:H13)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="14">
+      <c r="F14" s="42">
         <f t="shared" si="0"/>
         <v>87</v>
       </c>
-      <c r="F14" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="11">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B15" s="56">
+        <v>12</v>
+      </c>
+      <c r="C15" s="57">
         <v>45201</v>
       </c>
-      <c r="C15" s="14">
+      <c r="D15" s="42">
         <v>6</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <f>SUM(Calendar!B14:H14)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="14">
+      <c r="F15" s="42">
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
-      <c r="F15" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="68">
-        <v>10</v>
-      </c>
-      <c r="B16" s="11">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B16" s="56">
+        <v>13</v>
+      </c>
+      <c r="C16" s="57">
         <v>45208</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>15</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <f>SUM(Calendar!B15:H15)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="F16" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" s="10">
-        <v>11</v>
-      </c>
-      <c r="B17" s="11">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B17" s="56">
+        <v>14</v>
+      </c>
+      <c r="C17" s="57">
         <v>45215</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>5</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <f>SUM(Calendar!B16:H16)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="F17" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="10">
-        <v>12</v>
-      </c>
-      <c r="B18" s="11">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B18" s="56">
+        <v>15</v>
+      </c>
+      <c r="C18" s="57">
         <v>45222</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>5</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <f>SUM(Calendar!B17:H17)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="F18" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A19" s="10">
-        <v>13</v>
-      </c>
-      <c r="B19" s="11">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B19" s="56">
+        <v>16</v>
+      </c>
+      <c r="C19" s="57">
         <v>45229</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <v>5</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <f>SUM(Calendar!B18:H18)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="F19" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A20" s="10">
-        <v>14</v>
-      </c>
-      <c r="B20" s="11">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B20" s="56">
+        <v>17</v>
+      </c>
+      <c r="C20" s="57">
         <v>45236</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>5</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <f>SUM(Calendar!B19:H19)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="F20" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A21" s="68">
-        <v>15</v>
-      </c>
-      <c r="B21" s="11">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B21" s="56">
+        <v>18</v>
+      </c>
+      <c r="C21" s="57">
         <v>45243</v>
       </c>
-      <c r="C21" s="45">
+      <c r="D21" s="33">
         <v>20</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <f>SUM(Calendar!B20:H20)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="45">
+      <c r="F21" s="33">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F21" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A22" s="68">
-        <v>16</v>
-      </c>
-      <c r="B22" s="11">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B22" s="56">
+        <v>19</v>
+      </c>
+      <c r="C22" s="57">
         <v>45250</v>
       </c>
-      <c r="C22" s="15">
+      <c r="D22" s="12">
         <v>20</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <f>SUM(Calendar!B21:H21)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="15">
+      <c r="F22" s="12">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F22" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A23" s="68">
-        <v>17</v>
-      </c>
-      <c r="B23" s="11">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B23" s="56">
+        <v>20</v>
+      </c>
+      <c r="C23" s="57">
         <v>45257</v>
       </c>
-      <c r="C23" s="15">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1">
+      <c r="D23" s="12">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
         <f>SUM(Calendar!B22:H22)</f>
         <v>0</v>
       </c>
-      <c r="E23" s="15">
+      <c r="F23" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F23" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B24" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="13">
-        <f>SUM(C5:C23)</f>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B24" s="1"/>
+      <c r="C24" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="11">
+        <f>SUM(D5:D23)</f>
         <v>150</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A25" s="71"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="71"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="71"/>
-      <c r="K25" s="71"/>
-      <c r="L25" s="71"/>
-      <c r="M25" s="71"/>
-      <c r="N25" s="71"/>
-      <c r="O25" s="71"/>
-      <c r="P25" s="71"/>
-      <c r="Q25" s="72"/>
-      <c r="R25" s="36"/>
-    </row>
-    <row r="26" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A26" s="73" t="s">
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
+      <c r="O25" s="54"/>
+      <c r="P25" s="54"/>
+      <c r="Q25" s="54"/>
+      <c r="R25" s="55"/>
+      <c r="S25" s="32"/>
+    </row>
+    <row r="26" spans="1:19" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B26" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B27" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="73"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A27" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="53"/>
+      <c r="D27" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="42"/>
-      <c r="E27" s="41" t="s">
+      <c r="E27" s="52"/>
+      <c r="F27" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="42"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+      <c r="G27" s="52"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>0</v>
-      </c>
       <c r="D28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="G28" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A29" s="10">
+    <row r="29" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="59">
         <v>1</v>
       </c>
-      <c r="B29" s="11">
+      <c r="C29" s="57">
         <v>45131</v>
       </c>
-      <c r="C29" s="1">
-        <v>0</v>
-      </c>
       <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
         <f>SUM(Calendar!J4:P4)</f>
         <v>0</v>
       </c>
-      <c r="E29" s="1">
-        <f>C48</f>
+      <c r="F29" s="1">
+        <f>D48</f>
         <v>300</v>
       </c>
-      <c r="F29" s="1">
-        <f>C48</f>
+      <c r="G29" s="1">
+        <f>D48</f>
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A30" s="10">
+    <row r="30" spans="1:19" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="82">
         <v>2</v>
       </c>
-      <c r="B30" s="11">
+      <c r="C30" s="58">
         <v>45138</v>
       </c>
-      <c r="C30" s="1">
-        <v>0</v>
-      </c>
       <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
         <f>SUM(Calendar!J5:P5)</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="1">
-        <f>E29-C29</f>
-        <v>300</v>
+        <v>6</v>
       </c>
       <c r="F30" s="1">
         <f>F29-D29</f>
         <v>300</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A31" s="10">
+      <c r="G30" s="1">
+        <f>G29-E29</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B31" s="60">
         <v>3</v>
       </c>
-      <c r="B31" s="11">
+      <c r="C31" s="57">
         <v>45145</v>
       </c>
-      <c r="C31" s="1">
-        <v>0</v>
-      </c>
       <c r="D31" s="1">
+        <v>5</v>
+      </c>
+      <c r="E31" s="1">
         <f>SUM(Calendar!J6:P6)</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="1">
-        <f>E30-C30</f>
+        <v>5</v>
+      </c>
+      <c r="F31" s="1">
+        <f>F30-D30</f>
         <v>300</v>
       </c>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A32" s="10">
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B32" s="56">
         <v>4</v>
       </c>
-      <c r="B32" s="11">
+      <c r="C32" s="57">
         <v>45152</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="1">
+        <v>5</v>
+      </c>
+      <c r="E32" s="1">
+        <f>SUM(Calendar!J7:P7)</f>
+        <v>3</v>
+      </c>
+      <c r="F32" s="1">
+        <f>F31-D31</f>
+        <v>295</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B33" s="56">
+        <v>5</v>
+      </c>
+      <c r="C33" s="57">
+        <v>45159</v>
+      </c>
+      <c r="D33" s="1">
         <v>22</v>
       </c>
-      <c r="D32" s="1">
-        <f>SUM(Calendar!J7:P7)</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="1">
-        <f>E31-C31</f>
+      <c r="E33" s="1">
+        <f>SUM(Calendar!J8:P8)</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" ref="F33:F47" si="2">F32-D32</f>
+        <v>290</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B34" s="56">
+        <v>6</v>
+      </c>
+      <c r="C34" s="57">
+        <v>45166</v>
+      </c>
+      <c r="D34" s="1">
+        <v>22</v>
+      </c>
+      <c r="E34" s="1">
+        <f>SUM(Calendar!J9:P9)</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="2"/>
+        <v>268</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B35" s="56">
+        <v>7</v>
+      </c>
+      <c r="C35" s="57">
+        <v>45173</v>
+      </c>
+      <c r="D35" s="1">
+        <v>22</v>
+      </c>
+      <c r="E35" s="1">
+        <f>SUM(Calendar!J10:P10)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="2"/>
+        <v>246</v>
+      </c>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B36" s="56">
+        <v>8</v>
+      </c>
+      <c r="C36" s="57">
+        <v>45180</v>
+      </c>
+      <c r="D36" s="1">
+        <v>22</v>
+      </c>
+      <c r="E36" s="1">
+        <f>SUM(Calendar!J11:P11)</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="2"/>
+        <v>224</v>
+      </c>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B37" s="56">
+        <v>9</v>
+      </c>
+      <c r="C37" s="57">
+        <v>45187</v>
+      </c>
+      <c r="D37" s="1">
+        <v>23</v>
+      </c>
+      <c r="E37" s="1">
+        <f>SUM(Calendar!J12:P12)</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="2"/>
+        <v>202</v>
+      </c>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B38" s="56">
+        <v>10</v>
+      </c>
+      <c r="C38" s="57">
+        <v>45194</v>
+      </c>
+      <c r="D38" s="1">
+        <v>23</v>
+      </c>
+      <c r="E38" s="1">
+        <f>SUM(Calendar!J13:P13)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="42">
+        <f t="shared" si="2"/>
+        <v>179</v>
+      </c>
+      <c r="G38" s="42"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B39" s="56">
+        <v>11</v>
+      </c>
+      <c r="C39" s="57">
+        <v>45201</v>
+      </c>
+      <c r="D39" s="1">
+        <v>23</v>
+      </c>
+      <c r="E39" s="1">
+        <f>SUM(Calendar!J14:P14)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="42">
+        <f t="shared" si="2"/>
+        <v>156</v>
+      </c>
+      <c r="G39" s="42"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B40" s="56">
+        <v>12</v>
+      </c>
+      <c r="C40" s="57">
+        <v>45208</v>
+      </c>
+      <c r="D40" s="1">
+        <v>23</v>
+      </c>
+      <c r="E40" s="1">
+        <f>SUM(Calendar!J15:P15)</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="2"/>
+        <v>133</v>
+      </c>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B41" s="56">
+        <v>13</v>
+      </c>
+      <c r="C41" s="57">
+        <v>45215</v>
+      </c>
+      <c r="D41" s="1">
+        <v>22</v>
+      </c>
+      <c r="E41" s="1">
+        <f>SUM(Calendar!J16:P16)</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B42" s="56">
+        <v>14</v>
+      </c>
+      <c r="C42" s="57">
+        <v>45222</v>
+      </c>
+      <c r="D42" s="1">
+        <v>22</v>
+      </c>
+      <c r="E42" s="1">
+        <f>SUM(Calendar!J17:P17)</f>
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B43" s="56">
+        <v>15</v>
+      </c>
+      <c r="C43" s="57">
+        <v>45229</v>
+      </c>
+      <c r="D43" s="1">
+        <v>22</v>
+      </c>
+      <c r="E43" s="1">
+        <f>SUM(Calendar!J18:P18)</f>
+        <v>0</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B44" s="56">
+        <v>16</v>
+      </c>
+      <c r="C44" s="57">
+        <v>45236</v>
+      </c>
+      <c r="D44" s="1">
+        <v>22</v>
+      </c>
+      <c r="E44" s="1">
+        <f>SUM(Calendar!J19:P19)</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B45" s="56">
+        <v>17</v>
+      </c>
+      <c r="C45" s="57">
+        <v>45243</v>
+      </c>
+      <c r="D45" s="1">
+        <v>22</v>
+      </c>
+      <c r="E45" s="1">
+        <f>SUM(Calendar!J20:P20)</f>
+        <v>0</v>
+      </c>
+      <c r="F45" s="33">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="G45" s="33"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B46" s="56">
+        <v>18</v>
+      </c>
+      <c r="C46" s="57">
+        <v>45250</v>
+      </c>
+      <c r="D46" s="12">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1">
+        <f>SUM(Calendar!J21:P21)</f>
+        <v>0</v>
+      </c>
+      <c r="F46" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G46" s="12"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B47" s="56">
+        <v>19</v>
+      </c>
+      <c r="C47" s="57">
+        <v>45257</v>
+      </c>
+      <c r="D47" s="12">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1">
+        <f>SUM(Calendar!J22:P22)</f>
+        <v>0</v>
+      </c>
+      <c r="F47" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G47" s="12"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B48" s="1"/>
+      <c r="C48" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="1">
+        <f>SUM(D29:D47)</f>
         <v>300</v>
       </c>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="10">
-        <v>5</v>
-      </c>
-      <c r="B33" s="11">
-        <v>45159</v>
-      </c>
-      <c r="C33" s="1">
-        <v>22</v>
-      </c>
-      <c r="D33" s="1">
-        <f>SUM(Calendar!J8:P8)</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="1">
-        <f t="shared" ref="E33:E47" si="2">E32-C32</f>
-        <v>278</v>
-      </c>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="10">
-        <v>6</v>
-      </c>
-      <c r="B34" s="11">
-        <v>45166</v>
-      </c>
-      <c r="C34" s="1">
-        <v>22</v>
-      </c>
-      <c r="D34" s="1">
-        <f>SUM(Calendar!J9:P9)</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="1">
-        <f t="shared" si="2"/>
-        <v>256</v>
-      </c>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="10">
-        <v>7</v>
-      </c>
-      <c r="B35" s="11">
-        <v>45173</v>
-      </c>
-      <c r="C35" s="1">
-        <v>22</v>
-      </c>
-      <c r="D35" s="1">
-        <f>SUM(Calendar!J10:P10)</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="1">
-        <f t="shared" si="2"/>
-        <v>234</v>
-      </c>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="10">
-        <v>8</v>
-      </c>
-      <c r="B36" s="11">
-        <v>45180</v>
-      </c>
-      <c r="C36" s="1">
-        <v>22</v>
-      </c>
-      <c r="D36" s="1">
-        <f>SUM(Calendar!J11:P11)</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="1">
-        <f t="shared" si="2"/>
-        <v>212</v>
-      </c>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="10">
-        <v>9</v>
-      </c>
-      <c r="B37" s="11">
-        <v>45187</v>
-      </c>
-      <c r="C37" s="1">
-        <v>22</v>
-      </c>
-      <c r="D37" s="1">
-        <f>SUM(Calendar!J12:P12)</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="1">
-        <f t="shared" si="2"/>
-        <v>190</v>
-      </c>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="11">
-        <v>45194</v>
-      </c>
-      <c r="C38" s="1">
-        <v>21</v>
-      </c>
-      <c r="D38" s="1">
-        <f>SUM(Calendar!J13:P13)</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="14">
-        <f t="shared" si="2"/>
-        <v>168</v>
-      </c>
-      <c r="F38" s="14"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="11">
-        <v>45201</v>
-      </c>
-      <c r="C39" s="1">
-        <v>21</v>
-      </c>
-      <c r="D39" s="1">
-        <f>SUM(Calendar!J14:P14)</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="14">
-        <f t="shared" si="2"/>
-        <v>147</v>
-      </c>
-      <c r="F39" s="14"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="10">
-        <v>10</v>
-      </c>
-      <c r="B40" s="11">
-        <v>45208</v>
-      </c>
-      <c r="C40" s="1">
-        <v>21</v>
-      </c>
-      <c r="D40" s="1">
-        <f>SUM(Calendar!J15:P15)</f>
-        <v>0</v>
-      </c>
-      <c r="E40" s="1">
-        <f t="shared" si="2"/>
-        <v>126</v>
-      </c>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="10">
-        <v>11</v>
-      </c>
-      <c r="B41" s="11">
-        <v>45215</v>
-      </c>
-      <c r="C41" s="1">
-        <v>21</v>
-      </c>
-      <c r="D41" s="1">
-        <f>SUM(Calendar!J16:P16)</f>
-        <v>0</v>
-      </c>
-      <c r="E41" s="1">
-        <f t="shared" si="2"/>
-        <v>105</v>
-      </c>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="10">
-        <v>12</v>
-      </c>
-      <c r="B42" s="11">
-        <v>45222</v>
-      </c>
-      <c r="C42" s="1">
-        <v>21</v>
-      </c>
-      <c r="D42" s="1">
-        <f>SUM(Calendar!J17:P17)</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="1">
-        <f t="shared" si="2"/>
-        <v>84</v>
-      </c>
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="10">
-        <v>13</v>
-      </c>
-      <c r="B43" s="11">
-        <v>45229</v>
-      </c>
-      <c r="C43" s="1">
-        <v>21</v>
-      </c>
-      <c r="D43" s="1">
-        <f>SUM(Calendar!J18:P18)</f>
-        <v>0</v>
-      </c>
-      <c r="E43" s="1">
-        <f t="shared" si="2"/>
-        <v>63</v>
-      </c>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" s="10">
-        <v>14</v>
-      </c>
-      <c r="B44" s="11">
-        <v>45236</v>
-      </c>
-      <c r="C44" s="1">
-        <v>21</v>
-      </c>
-      <c r="D44" s="1">
-        <f>SUM(Calendar!J19:P19)</f>
-        <v>0</v>
-      </c>
-      <c r="E44" s="1">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="10">
-        <v>15</v>
-      </c>
-      <c r="B45" s="11">
-        <v>45243</v>
-      </c>
-      <c r="C45" s="1">
-        <v>21</v>
-      </c>
-      <c r="D45" s="1">
-        <f>SUM(Calendar!J20:P20)</f>
-        <v>0</v>
-      </c>
-      <c r="E45" s="45">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="F45" s="45"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="10">
-        <v>16</v>
-      </c>
-      <c r="B46" s="11">
-        <v>45250</v>
-      </c>
-      <c r="C46" s="15">
-        <v>0</v>
-      </c>
-      <c r="D46" s="1">
-        <f>SUM(Calendar!J21:P21)</f>
-        <v>0</v>
-      </c>
-      <c r="E46" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F46" s="15"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="10">
-        <v>17</v>
-      </c>
-      <c r="B47" s="11">
-        <v>45257</v>
-      </c>
-      <c r="C47" s="15">
-        <v>0</v>
-      </c>
-      <c r="D47" s="1">
-        <f>SUM(Calendar!J22:P22)</f>
-        <v>0</v>
-      </c>
-      <c r="E47" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F47" s="15"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B48" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" s="1">
-        <f>SUM(C29:C47)</f>
-        <v>300</v>
-      </c>
-      <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A25:Q25"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A2:F2"/>
+  <mergeCells count="11">
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="B1:R1"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B25:R25"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD3A90E3-FE87-4BB6-A9BE-2D3469258ACC}">
+  <dimension ref="B1:E29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="35.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="87"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="85"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="85"/>
+    </row>
+    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="92"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="85"/>
+    </row>
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="72" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="78"/>
+    </row>
+    <row r="7" spans="2:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="73">
+        <v>1</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="79"/>
+    </row>
+    <row r="8" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="B8" s="74">
+        <v>2</v>
+      </c>
+      <c r="C8" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="81" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="79"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="74">
+        <v>3</v>
+      </c>
+      <c r="C9" s="74"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="79"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="74">
+        <v>4</v>
+      </c>
+      <c r="C10" s="74"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="79"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="79"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="79"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="79"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="79"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="80"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="80"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="75"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="80"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="80"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="80"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" s="75"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="80"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="80"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="80"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="80"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="80"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="80"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="80"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="65"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="65"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="65"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>